<commit_message>
Update survey test to get input data from excel
</commit_message>
<xml_diff>
--- a/properties/testdata/Survey_TestData.xlsx
+++ b/properties/testdata/Survey_TestData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dung Bien\eclipse-workspace\mobilesitesurveytestautomation\properties\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{74891B22-5AC5-4AA7-91FC-8E847AA68B53}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EFC81B1E-CEE6-4F51-8B9F-D049EDCA98E9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9216" xr2:uid="{C2ED06FA-14B7-4F42-97B9-960AB2AAEA94}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FRB_Budget" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -706,8 +706,8 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,7 +1395,7 @@
         <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
         <v>84</v>

</xml_diff>